<commit_message>
* fix bug on build.gradle about labels generation. * update some packages (npm cache clean --force) * just for recording on VeeValidate issue.
</commit_message>
<xml_diff>
--- a/meta/labels/en/LabelsEn.xlsx
+++ b/meta/labels/en/LabelsEn.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10520"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yhaino/Desktop/dapanda-front-core/meta/labels/en/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/dapanda/dapanda-front-core/meta/labels/en/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED67CBFE-2FDD-6048-95DE-8E38DC015797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1B55E38-1E08-0F45-8C91-E501CD5C43EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="500" windowWidth="25520" windowHeight="15540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -377,7 +377,7 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>import {LocaleLabels} from "@/i18n/LocaleLabels";</t>
+    <t>import {LocaleLabels} from "@/i18n/LocaleLabels"</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -1659,7 +1659,7 @@
   </sheetPr>
   <dimension ref="A1:O65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
       <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>

</xml_diff>